<commit_message>
UserDAO 예외사항정리 완료_ DailyDAO, ManualDAO, StaffDAO 수정필요
</commit_message>
<xml_diff>
--- a/예외사항정리.xlsx
+++ b/예외사항정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB736364-B135-4FA0-9327-4800C531A396}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABECE8-30B8-4441-A48F-7695FECCC5B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="19390" windowHeight="7850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
   <si>
     <t>UserDAO.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,6 +394,86 @@
   </si>
   <si>
     <t>DailyDAOUnitTest참고 - removeDailyTaskWorngWithAssignDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패스워드 불일치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 재설정 시 양식 제한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDAOUnitTest - resetPwWithWrongFormat 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디에 해당하는 휴대폰 번호 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린아이디로 회원정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDAOUnitTest - setUserInfoWithWrongId 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원회원인증/회원정보변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디에 해당하는 회원정보 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린 아이디 - UserDAOUnitTest - getUserPhoneNumWithWrongId 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린 아이디 - UserDAOUnitTest - getUserInfoWithWrongId 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 변경 시 기존 비밀번호가 틀릴 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린 아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDAOUnitTest - setPwWithWrongOldPw 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>removeUserWithWrongId - setPwWithWrongOldPw 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린아이디로 슬라이드 메뉴 정보 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDAOUnitTest - getAdminSlideInfoWithWrongId 참고</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,7 +538,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -481,6 +561,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -821,11 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -867,73 +953,63 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -941,13 +1017,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -958,10 +1034,10 @@
         <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -969,41 +1045,41 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1011,328 +1087,468 @@
         <v>0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>30</v>
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="3" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="3" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3" t="s">
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="6" t="s">
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
+    <row r="49" spans="1:4" ht="85" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
+    <row r="50" spans="1:4" ht="85" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
+    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily, Manual, User DAO unit test 완료 / 비기능 예외사항 정리 완료 / StaffDAO Unit Test 추가 필요
</commit_message>
<xml_diff>
--- a/예외사항정리.xlsx
+++ b/예외사항정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABECE8-30B8-4441-A48F-7695FECCC5B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818D08C-CEB5-44C4-BCB9-2AEA2A78A314}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="19390" windowHeight="7850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="137">
   <si>
     <t>UserDAO.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,14 +297,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>위,위 내용과 비슷. 없는 파트에 업무배정 exception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위,위 내용과 비슷. 없는 개인에 업무배정 exception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - addDailyTaskWithWrongStaff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -373,22 +365,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>없는 업무 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - removeDailyTaskWorngWithNonExistDailyTask</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> assign_type 다른경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assign_detail 다른경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - removeDailyTaskWorngWithAssignType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -474,6 +454,133 @@
   </si>
   <si>
     <t>UserDAOUnitTest - getAdminSlideInfoWithWrongId 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자,직원,미인증자 여부확인</t>
+  </si>
+  <si>
+    <t>관리자/직원회원인증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디로 인증정보 확인 UserDAOUnitTest - getCertifiedInfo 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTaskTypesWrongWithNonExistSpaceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getSpaceTypesWrongWithNonExistTaskType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTasksWrongWithNonExistSpaceTypeTaskType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getManualTaskSeqWrongWithNonExistTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 공간분류에 해당하는 매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 업무분류에 해당하는 공간분류 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 공간분류, 없는 업무분류에 해당하는 매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 업무에 해당하는 매뉴얼 업무 SEQ찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간분류 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매뉴얼 업무 SEQ찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 날짜에 해당하는 배정대상 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAssignedPartsWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDailyTasksForPartsWrongWithAssignDateAssignDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDailyTasksForPersonWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파트별 - 선택한 날짜, 배정대상에 해당하는 업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인별 - 선택한 날짜에 해당하는 업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDailyTaskWithExistDailyTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배정날짜와 업무명이 중복되는 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDailyTaskWithWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는날짜에 업무명 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 파트에 업무배정 exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 개인에 업무배정 exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 삭제 - 없는 업무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무삭제 - assign_type다른경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무삭제 - assign_detail다른경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배정대상 목록보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 중복 확인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -907,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -957,10 +1064,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D4" s="9"/>
     </row>
@@ -969,10 +1076,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -1101,13 +1208,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -1115,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1129,13 +1236,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1160,10 +1267,10 @@
         <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -1174,10 +1281,10 @@
         <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -1188,10 +1295,10 @@
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.45">
@@ -1199,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
@@ -1227,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>105</v>
@@ -1236,32 +1343,32 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1272,13 +1379,13 @@
         <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
@@ -1286,10 +1393,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1297,13 +1404,13 @@
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1311,13 +1418,13 @@
         <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1325,55 +1432,55 @@
         <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
@@ -1381,13 +1488,13 @@
         <v>22</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -1395,41 +1502,41 @@
         <v>22</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.45">
@@ -1437,27 +1544,27 @@
         <v>22</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
@@ -1465,13 +1572,13 @@
         <v>22</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -1479,76 +1586,208 @@
         <v>22</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A52" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" s="6" t="s">
+      <c r="B52" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A53" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A54" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A55" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A49" s="3" t="s">
+    <row r="58" spans="1:4" ht="85" x14ac:dyDescent="0.45">
+      <c r="A58" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A50" s="3" t="s">
+    <row r="59" spans="1:4" ht="85" x14ac:dyDescent="0.45">
+      <c r="A59" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.45">
-      <c r="A51" s="3" t="s">
+    <row r="60" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+      <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
develop 업데이트 --> yunjin branch
</commit_message>
<xml_diff>
--- a/예외사항정리.xlsx
+++ b/예외사항정리.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABECE8-30B8-4441-A48F-7695FECCC5B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{842214C4-7F5E-4521-B46A-6B659D334A4C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="19390" windowHeight="7850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="19395" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="190">
   <si>
     <t>UserDAO.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,14 +297,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>위,위 내용과 비슷. 없는 파트에 업무배정 exception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위,위 내용과 비슷. 없는 개인에 업무배정 exception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - addDailyTaskWithWrongStaff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -373,22 +365,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>없는 업무 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - removeDailyTaskWorngWithNonExistDailyTask</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> assign_type 다른경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assign_detail 다른경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DailyDAOUnitTest참고 - removeDailyTaskWorngWithAssignType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -475,6 +455,307 @@
   <si>
     <t>UserDAOUnitTest - getAdminSlideInfoWithWrongId 참고</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자,직원,미인증자 여부확인</t>
+  </si>
+  <si>
+    <t>관리자/직원회원인증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디로 인증정보 확인 UserDAOUnitTest - getCertifiedInfo 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTaskTypesWrongWithNonExistSpaceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getSpaceTypesWrongWithNonExistTaskType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTasksWrongWithNonExistSpaceTypeTaskType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getManualTaskSeqWrongWithNonExistTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 공간분류에 해당하는 매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 업무분류에 해당하는 공간분류 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 공간분류, 없는 업무분류에 해당하는 매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 업무에 해당하는 매뉴얼 업무 SEQ찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매뉴얼 업무 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간분류 전체 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매뉴얼 업무 SEQ찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 날짜에 해당하는 배정대상 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAssignedPartsWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDailyTasksForPartsWrongWithAssignDateAssignDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDailyTasksForPersonWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파트별 - 선택한 날짜, 배정대상에 해당하는 업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인별 - 선택한 날짜에 해당하는 업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDailyTaskWithExistDailyTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배정날짜와 업무명이 중복되는 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDailyTaskWithWrongWithAssignDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는날짜에 업무명 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 파트에 업무배정 exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 개인에 업무배정 exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 삭제 - 없는 업무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무삭제 - assign_type다른경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무삭제 - assign_detail다른경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배정대상 목록보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 목록 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점코드 입력 가능범위 초과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getWorkPartsWithOutofboundsBranchSeq</t>
+  </si>
+  <si>
+    <t>직원 소속파트 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없는 지점의 소속파트 가져오기</t>
+  </si>
+  <si>
+    <t>getWorkPartsWithWrongBranchSeq</t>
+  </si>
+  <si>
+    <t>없는 지점의 직원목록 가져오기</t>
+  </si>
+  <si>
+    <t>직원 목록 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getWorkingStaffsWithWrongBranchSeq</t>
+  </si>
+  <si>
+    <t>없는 지점의 직원 인증요청 목록 가져오기</t>
+  </si>
+  <si>
+    <t>getPreStaffsWithNonexistBranchSeq</t>
+  </si>
+  <si>
+    <t>직원 인증요청 목록 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 인증요청 수락한(재직중인) 직원을 재수락하는 경우</t>
+  </si>
+  <si>
+    <t>setJoinDateWithPreStaff</t>
+  </si>
+  <si>
+    <t>직원 인증요청 수락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증요청하지 않은 직원의 입사일을 등록하는 경우(회원이지만 인증요청X or 비회원)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setJoinDateWithoutAddStaff</t>
+  </si>
+  <si>
+    <t>이미 퇴사한 직원을 퇴사시키려는 경우-예외처리 필요</t>
+  </si>
+  <si>
+    <t>직원 인증요청 거부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴사 직원 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setLeaveDateWithLeftStaff</t>
+  </si>
+  <si>
+    <t>인증요청만 하고 승인 안 된 직원을 퇴사시키는 경우</t>
+  </si>
+  <si>
+    <t>setLeaveDateWithPreStaff</t>
+  </si>
+  <si>
+    <t>인증요청하지 않은 직원의 퇴사일을 등록하는 경우/존재하지 않는 회원의 경우</t>
+  </si>
+  <si>
+    <t>setLeaveDateWithWrongStaff</t>
+  </si>
+  <si>
+    <t>getLeftStaffsWithWrongBranchSeq</t>
+  </si>
+  <si>
+    <t>없는 지점의 퇴사직원 목록 조회</t>
+  </si>
+  <si>
+    <t>퇴사 직원 목록 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 상세 정보 보기</t>
+  </si>
+  <si>
+    <t>없는 지점의 직원 상세 보기</t>
+  </si>
+  <si>
+    <t>getStaffDetailWithWrongBranchSeq</t>
+  </si>
+  <si>
+    <t>없는 직원 상세 보기</t>
+  </si>
+  <si>
+    <t>getStaffDetailWithWrongStaffId</t>
+  </si>
+  <si>
+    <t>직원 등록(승인요청)</t>
+  </si>
+  <si>
+    <t>재직중인 직원인데 인증요청하는 경우(입사일을 덮어씌우는 경우)</t>
+  </si>
+  <si>
+    <t>addStaffWithJoinedStaff
+추가 예외처리 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증요청한 직원이 계속 인증요청 하는 경우</t>
+  </si>
+  <si>
+    <t>addStaffWithPreStaff
+추가 예외처리 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 회원정보 변경</t>
+  </si>
+  <si>
+    <t>setStaffInfoWithPreStaff</t>
+  </si>
+  <si>
+    <t>인증 승인 대기중인 직원의 직원정보 변경-UI에서 할 수가 없음</t>
+  </si>
+  <si>
+    <t>없는 직원의 직원정보 변경</t>
+  </si>
+  <si>
+    <t>setStaffInfoWithWrongStaff</t>
+  </si>
+  <si>
+    <t>부적절한 파일형식으로 변경하는 경우</t>
+  </si>
+  <si>
+    <t>setStaffInfoWithWrongFileFormat</t>
+  </si>
+  <si>
+    <t>부적절한 계좌번호 형식으로 변경하는 경우</t>
+  </si>
+  <si>
+    <t>setStaffInfoWithWrongAccountNumFormat</t>
+  </si>
+  <si>
+    <t>이미 승인 처리받은 직원(재직) 의 요청을 거부하려고 하는 경우</t>
+  </si>
+  <si>
+    <t>인증요청하지 않은 경우(or 없는 직원의 경우)</t>
+  </si>
+  <si>
+    <t>removeStaffWithJoinedStaff</t>
+  </si>
+  <si>
+    <t>removeStaffWithWrongStaffId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴사한 직원의 인증을 거부하는 경우</t>
+  </si>
+  <si>
+    <t>removeStaffWithLeftStaff</t>
   </si>
 </sst>
 </file>
@@ -907,23 +1188,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.9140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.4140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="78.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="78.625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -937,8 +1218,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.5" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -952,53 +1233,59 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1006,13 +1293,13 @@
         <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1020,27 +1307,27 @@
         <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,27 +1335,27 @@
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1076,69 +1363,69 @@
         <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
@@ -1146,13 +1433,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -1160,13 +1447,13 @@
         <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -1174,69 +1461,69 @@
         <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>22</v>
       </c>
@@ -1250,7 +1537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
@@ -1261,10 +1548,10 @@
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1278,278 +1565,700 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="6" t="s">
+      <c r="B51" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A49" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="3" t="s">
+    <row r="57" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="3" t="s">
+    <row r="58" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.45">
-      <c r="A51" s="3" t="s">
+    <row r="59" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1565,7 +2274,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1578,7 +2287,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>